<commit_message>
added new sensor migration and fixes to ble
</commit_message>
<xml_diff>
--- a/new_format.xlsx
+++ b/new_format.xlsx
@@ -442,8 +442,8 @@
   </sheetPr>
   <dimension ref="A2:U44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R40" activeCellId="0" sqref="R40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U18" activeCellId="0" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,6 +846,68 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H18" s="2" t="s">
@@ -1405,7 +1467,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1428,7 +1490,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>